<commit_message>
Revert "2023 11 28"
</commit_message>
<xml_diff>
--- a/doc/project-proposal/画面レイアウト図/画面レイアウト.xlsx
+++ b/doc/project-proposal/画面レイアウト図/画面レイアウト.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkat\Code\System-Development-Group-Exercise-2\doc\project-proposal\画面レイアウト図\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F94AF-9BBD-414E-9C87-EF68E3886912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF139C0C-9517-4973-9B71-89139FE2B59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19466" yWindow="0" windowWidth="13534" windowHeight="17880" xr2:uid="{6403D1D6-6A69-4038-B069-E4E41010E8BE}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{6403D1D6-6A69-4038-B069-E4E41010E8BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -56,6 +67,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>[LO01]Login.png</t>
+  </si>
+  <si>
+    <t>[SB01]SideBer.png</t>
+  </si>
+  <si>
     <t>[CH01]CheckIN_or_OUT.png</t>
   </si>
   <si>
@@ -83,6 +100,9 @@
     <t>[CI08]Customer_information_deletion_confirmation.png</t>
   </si>
   <si>
+    <t>[IR01]Invoices_or_Receipts.png</t>
+  </si>
+  <si>
     <t>[EI01]Employee_information.png</t>
   </si>
   <si>
@@ -108,6 +128,36 @@
   </si>
   <si>
     <t>[RoI08]Room_information_deletion_confirmation.png</t>
+  </si>
+  <si>
+    <t>[Pa01]Password_setting.png</t>
+  </si>
+  <si>
+    <t>[ReI01]Reservation_information.png</t>
+  </si>
+  <si>
+    <t>[ReI02]Reservation_information_search.png</t>
+  </si>
+  <si>
+    <t>[ReI03]Reservation_information_show.png</t>
+  </si>
+  <si>
+    <t>[ReI07]Reservation_information_registration_confirmation.png</t>
+  </si>
+  <si>
+    <t>[ReI08]Reservation_information_select.png</t>
+  </si>
+  <si>
+    <t>[ReI09]Reservation_information_change.png</t>
+  </si>
+  <si>
+    <t>[ReI10]Reservation_information_change_confirmation.png</t>
+  </si>
+  <si>
+    <t>[ReI11]Reservation_information_deletion_confirmation.png</t>
+  </si>
+  <si>
+    <t>[ReI13]Reservation_information_showlist.png</t>
   </si>
   <si>
     <t>[EI02]Employee_information_registration.png</t>
@@ -530,6 +580,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>[ReI12]Reservation_information_show_search.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>請求書・領収書画面</t>
+    <rPh sb="0" eb="3">
+      <t>セイキュウショ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>リョウシュウショ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>従業員情報画面</t>
     <rPh sb="0" eb="5">
       <t>ジュウギョウインジョウホウ</t>
@@ -722,95 +789,6 @@
     <rPh sb="8" eb="10">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>長谷川 日向</t>
-    <rPh sb="0" eb="3">
-      <t>ハセガワ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ヒナタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>印銀 克哉</t>
-    <rPh sb="0" eb="1">
-      <t>イン</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>ギン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>カツヤ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>長野 裕馬</t>
-    <rPh sb="0" eb="2">
-      <t>ナガノ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ユウマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[Pa01]Password_setting.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[SB01]SideBer.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI01]Reservation_information.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI02]Reservation_information_search.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI03]Reservation_information_show.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI05]Reservation_information_registration_confirmation.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI06]Reservation_information_select.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI07]Reservation_information_change.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI08]Reservation_information_change_confirmation.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI09]Reservation_information_deletion_confirmation.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI10]Reservation_information_show_search.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ReI11]Reservation_information_showlist.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[LO01]Login.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -857,7 +835,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -866,6 +844,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,17 +1162,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E705D5-0F73-44F2-8A42-1E885A83FAE9}">
-  <dimension ref="B2:D46"/>
+  <dimension ref="B2:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="2" max="2" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.0703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.78515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1202,456 +1183,399 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B31" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B5" t="s">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B21"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B22" t="s">
+      <c r="C39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B23" t="s">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B24" t="s">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B26" t="s">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B27" t="s">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B28" t="s">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C28" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B29" t="s">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B30" t="s">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B31" t="s">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.65">
+      <c r="B48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C31" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B33"/>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B38"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-      <c r="D41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B44" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B45" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" t="s">
-        <v>70</v>
-      </c>
+      <c r="D48" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>